<commit_message>
Added emumba site post flyer test
</commit_message>
<xml_diff>
--- a/src/test/resources/qaautomation.xlsx
+++ b/src/test/resources/qaautomation.xlsx
@@ -61,7 +61,7 @@
     <t xml:space="preserve">After Life (TV Series 2019– ) - IMDb</t>
   </si>
   <si>
-    <t xml:space="preserve">tony.way79@gmail.com</t>
+    <t xml:space="preserve">tony.way85@gmail.com</t>
   </si>
   <si>
     <t xml:space="preserve">Emumba Pvt. Limited, Korang Road I-10/3 Islamabad.</t>
@@ -713,7 +713,7 @@
       <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.53125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="24.81"/>
   </cols>
@@ -801,7 +801,7 @@
       <selection pane="topLeft" activeCell="H12" activeCellId="0" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.53125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="65.96"/>
   </cols>
@@ -923,7 +923,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.53125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
@@ -1133,7 +1133,7 @@
       <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.53125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">

</xml_diff>

<commit_message>
fixed dependency on manual email change
</commit_message>
<xml_diff>
--- a/src/test/resources/qaautomation.xlsx
+++ b/src/test/resources/qaautomation.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Input" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="875" uniqueCount="324">
   <si>
     <t xml:space="preserve">URL</t>
   </si>
@@ -61,7 +61,35 @@
     <t xml:space="preserve">After Life (TV Series 2019– ) - IMDb</t>
   </si>
   <si>
-    <t xml:space="preserve">tony.way88@gmail.com</t>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">tony.way</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">[@here]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">@gmail.com</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Emumba Pvt. Limited, Korang Road I-10/3 Islamabad.</t>
@@ -106,7 +134,7 @@
     <t xml:space="preserve">POST</t>
   </si>
   <si>
-    <t xml:space="preserve">{    "first_name": "Ali",    "last_name": "Ahmad",    "email": "ali.ahmad236@gmail.com",    "password": "12345",    "confirm_password": "12345"}</t>
+    <t xml:space="preserve">{    "first_name": "Ali",    "last_name": "Ahmad",    "email": "ali.ahmad23[@here]@gmail.com",    "password": "12345",    "confirm_password": "12345"}</t>
   </si>
   <si>
     <t xml:space="preserve">["email","first_name","last_name","plan","id","access_token","refresh_token"]</t>
@@ -1004,7 +1032,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -1026,6 +1054,12 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1102,8 +1136,8 @@
   </sheetPr>
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1140,7 +1174,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -1190,8 +1224,8 @@
   </sheetPr>
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>